<commit_message>
[FIX] sendsetting init data addUser modify
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-08-28-init-data.xlsx
+++ b/src/main/resources/script/db/2018-08-28-init-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="19425" tabRatio="987" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="19425" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -1944,14 +1944,6 @@
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
-    <t>添加/导入新用户</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>管理员添加或导入新用户时，新用户收到自己的账户信息</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
     <t>添加新功能</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
@@ -2245,6 +2237,14 @@
   </si>
   <si>
     <t>系统通知</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员添加/导入新用户</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员添加或导入新用户时，管理员收到添加用户结果的反馈</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
 </sst>
@@ -3211,8 +3211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D7:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3228,31 +3228,31 @@
   <sheetData>
     <row r="7" spans="4:12">
       <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" t="s">
         <v>57</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>58</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>59</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>60</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>61</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>62</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>63</v>
-      </c>
-      <c r="K7" t="s">
-        <v>64</v>
-      </c>
-      <c r="L7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="4:12">
@@ -3283,16 +3283,16 @@
     </row>
     <row r="9" spans="4:12">
       <c r="E9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="I9" t="s">
         <v>47</v>
@@ -3309,16 +3309,16 @@
     </row>
     <row r="10" spans="4:12">
       <c r="E10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
         <v>47</v>
@@ -3335,16 +3335,16 @@
     </row>
     <row r="11" spans="4:12">
       <c r="E11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I11" t="s">
         <v>47</v>
@@ -3361,19 +3361,19 @@
     </row>
     <row r="12" spans="4:12">
       <c r="E12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -3387,16 +3387,16 @@
     </row>
     <row r="13" spans="4:12">
       <c r="E13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I13" t="s">
         <v>47</v>
@@ -3413,16 +3413,16 @@
     </row>
     <row r="14" spans="4:12">
       <c r="E14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I14" t="s">
         <v>47</v>
@@ -3439,16 +3439,16 @@
     </row>
     <row r="15" spans="4:12">
       <c r="E15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I15" t="s">
         <v>47</v>
@@ -3474,7 +3474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D7:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -3491,31 +3491,31 @@
   <sheetData>
     <row r="7" spans="4:17">
       <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
         <v>66</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" t="s">
         <v>67</v>
       </c>
-      <c r="F7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
         <v>68</v>
       </c>
-      <c r="H7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>69</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>70</v>
-      </c>
-      <c r="K7" t="s">
-        <v>71</v>
-      </c>
-      <c r="L7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="8" spans="4:17">
@@ -3523,25 +3523,25 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O8" s="28"/>
       <c r="Q8" s="28"/>
@@ -3551,25 +3551,25 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="4:17">
@@ -3577,25 +3577,25 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="4:17">
@@ -3603,25 +3603,25 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="4:17">
@@ -3629,25 +3629,25 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="4:17">
@@ -3655,25 +3655,25 @@
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="4:17">
@@ -3681,25 +3681,25 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="4:17">
@@ -3707,25 +3707,25 @@
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ADD] add receiveSetting controller;modify notice send and add receive config;remove send setting organization and modify send setting site.
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-08-28-init-data.xlsx
+++ b/src/main/resources/script/db/2018-08-28-init-data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcalaz/work/code/choerodon/notify-service/src/main/resources/script/db/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DYQ\tranning\choerodon-framework\notify-service\src\main\resources\script\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF799D49-1812-4675-AAAB-ADBFE28180BD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="19425" tabRatio="987" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="139">
   <si>
     <r>
       <rPr>
@@ -2078,10 +2079,6 @@
     <t>&lt;p&gt;您好，&lt;/p&gt;&lt;p&gt;您所在的项目：${projectName} 已被启用。&lt;/p&gt;</t>
   </si>
   <si>
-    <t>site</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
     <t>停用项目</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
@@ -2253,10 +2250,6 @@
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
-    <t>site</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
     <t>forgetPassword-preset</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
@@ -2294,14 +2287,26 @@
   </si>
   <si>
     <t>用户注册组织，发送邮箱验证进行验证</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>IS_ALLOW_CONFIG</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>organization</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>project</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2666,7 +2671,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="1"/>
+    <cellStyle name="Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3007,21 +3012,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="9" style="5"/>
-    <col min="3" max="3" width="100.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="63.95" customHeight="1">
       <c r="A1" s="6"/>
       <c r="C1" s="30" t="s">
         <v>0</v>
@@ -3032,12 +3037,12 @@
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2"/>
       <c r="D2"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="48.95" customHeight="1">
       <c r="A3"/>
       <c r="C3" s="29" t="s">
         <v>1</v>
@@ -3049,7 +3054,7 @@
       <c r="F3" s="31"/>
       <c r="G3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="31.5">
       <c r="A4"/>
       <c r="C4" s="32" t="s">
         <v>3</v>
@@ -3065,17 +3070,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="6"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
@@ -3086,7 +3091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
@@ -3095,7 +3100,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="173.25">
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
@@ -3109,7 +3114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="204.75">
       <c r="C10" s="13" t="s">
         <v>17</v>
       </c>
@@ -3120,7 +3125,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="85.5" customHeight="1">
       <c r="C11" s="9" t="s">
         <v>20</v>
       </c>
@@ -3131,7 +3136,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="47.25">
       <c r="C12" s="9" t="s">
         <v>23</v>
       </c>
@@ -3142,17 +3147,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:8" ht="138" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="132.75">
       <c r="C15" s="14" t="s">
         <v>26</v>
       </c>
@@ -3163,26 +3168,26 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="D16"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:5">
       <c r="D17"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:5">
       <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D18"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:5">
       <c r="C19" s="33" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:5">
       <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
@@ -3190,7 +3195,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:5">
       <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
@@ -3198,7 +3203,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:5">
       <c r="C22" s="3" t="s">
         <v>33</v>
       </c>
@@ -3206,7 +3211,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:5">
       <c r="C23" s="3" t="s">
         <v>35</v>
       </c>
@@ -3214,10 +3219,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:5">
       <c r="D24"/>
     </row>
-    <row r="25" spans="3:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:5" ht="69" customHeight="1">
       <c r="C25" s="17" t="s">
         <v>37</v>
       </c>
@@ -3226,7 +3231,7 @@
       </c>
       <c r="E25" s="29"/>
     </row>
-    <row r="26" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:5" ht="15.75" customHeight="1">
       <c r="C26" s="10" t="s">
         <v>39</v>
       </c>
@@ -3235,7 +3240,7 @@
       </c>
       <c r="E26" s="29"/>
     </row>
-    <row r="27" spans="3:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:5" ht="31.5">
       <c r="C27" s="18" t="s">
         <v>41</v>
       </c>
@@ -3257,25 +3262,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D7:L16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="D7:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="68" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.125" customWidth="1"/>
+    <col min="5" max="6" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.125" customWidth="1"/>
+    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="4:13">
       <c r="D7" t="s">
         <v>55</v>
       </c>
@@ -3303,8 +3309,11 @@
       <c r="L7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="4:13">
       <c r="E8" t="s">
         <v>44</v>
       </c>
@@ -3329,8 +3338,11 @@
       <c r="L8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:13">
       <c r="E9" t="s">
         <v>52</v>
       </c>
@@ -3338,13 +3350,13 @@
         <v>52</v>
       </c>
       <c r="G9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" t="s">
         <v>122</v>
       </c>
-      <c r="H9" t="s">
-        <v>123</v>
-      </c>
       <c r="I9" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -3355,8 +3367,11 @@
       <c r="L9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="4:13">
       <c r="E10" t="s">
         <v>53</v>
       </c>
@@ -3381,8 +3396,11 @@
       <c r="L10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13">
       <c r="E11" t="s">
         <v>54</v>
       </c>
@@ -3407,22 +3425,25 @@
       <c r="L11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="4:13">
       <c r="E12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -3433,22 +3454,25 @@
       <c r="L12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:13">
       <c r="E13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
         <v>90</v>
       </c>
-      <c r="F13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" t="s">
-        <v>91</v>
-      </c>
       <c r="I13" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -3459,22 +3483,25 @@
       <c r="L13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="4:13">
       <c r="E14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I14" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -3485,22 +3512,25 @@
       <c r="L14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="4:13">
       <c r="E15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -3511,22 +3541,25 @@
       <c r="L15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="4:13">
       <c r="E16" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" t="s">
         <v>125</v>
       </c>
-      <c r="F16" t="s">
-        <v>124</v>
-      </c>
-      <c r="G16" t="s">
-        <v>126</v>
-      </c>
       <c r="H16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I16" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -3536,6 +3569,9 @@
       </c>
       <c r="L16">
         <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3546,27 +3582,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D7:R16"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8:K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.1640625" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="109.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.125" customWidth="1"/>
+    <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="109.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="4:18">
       <c r="D7" t="s">
         <v>64</v>
       </c>
@@ -3589,7 +3625,7 @@
         <v>68</v>
       </c>
       <c r="K7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L7" t="s">
         <v>69</v>
@@ -3598,15 +3634,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:18">
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s">
         <v>72</v>
@@ -3615,7 +3651,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L8" t="s">
         <v>76</v>
@@ -3626,15 +3662,15 @@
       <c r="P8" s="28"/>
       <c r="R8" s="28"/>
     </row>
-    <row r="9" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:18">
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H9" t="s">
         <v>73</v>
@@ -3643,7 +3679,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L9" t="s">
         <v>77</v>
@@ -3652,15 +3688,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:18">
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H10" t="s">
         <v>72</v>
@@ -3669,7 +3705,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L10" t="s">
         <v>75</v>
@@ -3678,15 +3714,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="4:18">
       <c r="E11">
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H11" t="s">
         <v>73</v>
@@ -3695,7 +3731,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L11" t="s">
         <v>74</v>
@@ -3704,15 +3740,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="4:18">
       <c r="E12">
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H12" t="s">
         <v>72</v>
@@ -3721,123 +3757,123 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L12" t="s">
         <v>102</v>
       </c>
-      <c r="L12" t="s">
-        <v>103</v>
-      </c>
       <c r="M12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="4:18" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="4:18">
       <c r="E13">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="4:18" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="4:18">
       <c r="E14">
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="4:18" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="4:18">
       <c r="E15">
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L15" t="s">
+        <v>109</v>
+      </c>
+      <c r="M15" t="s">
         <v>110</v>
       </c>
-      <c r="M15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="4:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="4:18">
       <c r="E16">
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] fix email record template,receive setting;
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-08-28-init-data.xlsx
+++ b/src/main/resources/script/db/2018-08-28-init-data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcalaz/work/code/choerodon/notify-service/src/main/resources/script/db/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DYQ\tranning\choerodon-framework\notify-service\src\main\resources\script\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5B7272-5C5D-4D5B-AE2B-CF435963CCB4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16760" windowHeight="21000" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="21000" tabRatio="987" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="139">
   <si>
     <r>
       <rPr>
@@ -2298,86 +2299,14 @@
   </si>
   <si>
     <t>project</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>issueCreate</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>问题创建</t>
-    <rPh sb="0" eb="1">
-      <t>wen t</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>chuang jian</t>
-    </rPh>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>问题创建，给相关用户发送通知</t>
-    <rPh sb="5" eb="6">
-      <t>gei</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>xiang guan</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>yong hu</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>fa song</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>tong zhi</t>
-    </rPh>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>issueAssignee</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>问题分配</t>
-    <rPh sb="0" eb="1">
-      <t>wen ti</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>fen pei</t>
-    </rPh>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>问题分配，给相关用户发送通知</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>issueSolve</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>问题已解决</t>
-    <rPh sb="0" eb="1">
-      <t>wen ti</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>yi jing</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>jie jue</t>
-    </rPh>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>问题已解决，给相关用户发送通知</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2742,7 +2671,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="1"/>
+    <cellStyle name="Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3083,21 +3012,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="9" style="5"/>
-    <col min="3" max="3" width="100.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="63.95" customHeight="1">
       <c r="A1" s="6"/>
       <c r="C1" s="30" t="s">
         <v>0</v>
@@ -3108,12 +3037,12 @@
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2"/>
       <c r="D2"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="48.95" customHeight="1">
       <c r="A3"/>
       <c r="C3" s="29" t="s">
         <v>1</v>
@@ -3125,7 +3054,7 @@
       <c r="F3" s="31"/>
       <c r="G3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="31.5">
       <c r="A4"/>
       <c r="C4" s="32" t="s">
         <v>3</v>
@@ -3141,17 +3070,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="6"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
@@ -3162,7 +3091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
@@ -3171,7 +3100,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="173.25">
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
@@ -3185,7 +3114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="204.75">
       <c r="C10" s="13" t="s">
         <v>17</v>
       </c>
@@ -3196,7 +3125,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="85.5" customHeight="1">
       <c r="C11" s="9" t="s">
         <v>20</v>
       </c>
@@ -3207,7 +3136,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="47.25">
       <c r="C12" s="9" t="s">
         <v>23</v>
       </c>
@@ -3218,17 +3147,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:8" ht="138" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="132.75">
       <c r="C15" s="14" t="s">
         <v>26</v>
       </c>
@@ -3239,26 +3168,26 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="D16"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:5">
       <c r="D17"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:5">
       <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D18"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:5">
       <c r="C19" s="33" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:5">
       <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
@@ -3266,7 +3195,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:5">
       <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
@@ -3274,7 +3203,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:5">
       <c r="C22" s="3" t="s">
         <v>33</v>
       </c>
@@ -3282,7 +3211,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:5">
       <c r="C23" s="3" t="s">
         <v>35</v>
       </c>
@@ -3290,10 +3219,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:5">
       <c r="D24"/>
     </row>
-    <row r="25" spans="3:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:5" ht="69" customHeight="1">
       <c r="C25" s="17" t="s">
         <v>37</v>
       </c>
@@ -3302,7 +3231,7 @@
       </c>
       <c r="E25" s="29"/>
     </row>
-    <row r="26" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:5" ht="15.75" customHeight="1">
       <c r="C26" s="10" t="s">
         <v>39</v>
       </c>
@@ -3311,7 +3240,7 @@
       </c>
       <c r="E26" s="29"/>
     </row>
-    <row r="27" spans="3:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:5" ht="31.5">
       <c r="C27" s="18" t="s">
         <v>41</v>
       </c>
@@ -3333,26 +3262,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D7:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1640625" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.125" customWidth="1"/>
+    <col min="5" max="6" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.125" customWidth="1"/>
+    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="4:13">
       <c r="D7" t="s">
         <v>55</v>
       </c>
@@ -3384,7 +3313,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:13">
       <c r="E8" t="s">
         <v>44</v>
       </c>
@@ -3413,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:13">
       <c r="E9" t="s">
         <v>52</v>
       </c>
@@ -3442,7 +3371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:13">
       <c r="E10" t="s">
         <v>53</v>
       </c>
@@ -3471,7 +3400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="4:13">
       <c r="E11" t="s">
         <v>54</v>
       </c>
@@ -3500,7 +3429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="4:13">
       <c r="E12" t="s">
         <v>88</v>
       </c>
@@ -3529,7 +3458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="4:13">
       <c r="E13" t="s">
         <v>89</v>
       </c>
@@ -3558,7 +3487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="4:13">
       <c r="E14" t="s">
         <v>86</v>
       </c>
@@ -3587,7 +3516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="4:13">
       <c r="E15" t="s">
         <v>87</v>
       </c>
@@ -3616,7 +3545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="4:13">
       <c r="E16" t="s">
         <v>124</v>
       </c>
@@ -3645,25 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E17" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G17" t="s">
-        <v>140</v>
-      </c>
-      <c r="H17" t="s">
-        <v>141</v>
-      </c>
-      <c r="I17" t="s">
-        <v>47</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
+    <row r="17" spans="11:13">
       <c r="K17">
         <v>1</v>
       </c>
@@ -3674,25 +3585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F18" t="s">
-        <v>142</v>
-      </c>
-      <c r="G18" t="s">
-        <v>143</v>
-      </c>
-      <c r="H18" t="s">
-        <v>144</v>
-      </c>
-      <c r="I18" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
+    <row r="18" spans="11:13">
       <c r="K18">
         <v>1</v>
       </c>
@@ -3703,25 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E19" t="s">
-        <v>145</v>
-      </c>
-      <c r="F19" t="s">
-        <v>145</v>
-      </c>
-      <c r="G19" t="s">
-        <v>146</v>
-      </c>
-      <c r="H19" t="s">
-        <v>147</v>
-      </c>
-      <c r="I19" t="s">
-        <v>47</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
+    <row r="19" spans="11:13">
       <c r="K19">
         <v>1</v>
       </c>
@@ -3740,27 +3615,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D7:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.1640625" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="109.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.125" customWidth="1"/>
+    <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="109.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="4:18">
       <c r="D7" t="s">
         <v>64</v>
       </c>
@@ -3792,7 +3667,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:18">
       <c r="E8">
         <v>1</v>
       </c>
@@ -3820,7 +3695,7 @@
       <c r="P8" s="28"/>
       <c r="R8" s="28"/>
     </row>
-    <row r="9" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:18">
       <c r="E9">
         <v>2</v>
       </c>
@@ -3846,7 +3721,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:18">
       <c r="E10">
         <v>3</v>
       </c>
@@ -3872,7 +3747,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="4:18">
       <c r="E11">
         <v>4</v>
       </c>
@@ -3898,7 +3773,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="4:18">
       <c r="E12">
         <v>5</v>
       </c>
@@ -3924,7 +3799,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="4:18">
       <c r="E13">
         <v>6</v>
       </c>
@@ -3950,7 +3825,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="4:18">
       <c r="E14">
         <v>7</v>
       </c>
@@ -3976,7 +3851,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="4:18">
       <c r="E15">
         <v>8</v>
       </c>
@@ -4005,7 +3880,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="4:18">
       <c r="E16">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
[FIX] fix email template init-data;
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-08-28-init-data.xlsx
+++ b/src/main/resources/script/db/2018-08-28-init-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DYQ\tranning\choerodon-framework\notify-service\src\main\resources\script\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B42BEE-F145-4F51-A3BA-357AC49AD1E8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2987A569-F5D8-47C9-83CD-4740EF58DA38}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="21000" tabRatio="987" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="21000" tabRatio="987" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="137">
   <si>
     <r>
       <rPr>
@@ -2184,85 +2184,107 @@
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
-    <t>验证邮件</t>
+    <t>停用组织</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加新用户</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改密码</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>pm</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>addFunction</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>addFunction-preset</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;p&gt;您已经成功添加${addCount}名新用户&lt;/p&gt;</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>${content}</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统通知</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统通知</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员添加/导入新用户</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员添加或导入新用户时，管理员收到添加用户结果的反馈</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>registerOrganization</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>registerOrganization</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册组织</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>forgetPassword-preset</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>registerOrganization-preset</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>enableOrganization</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>registerOrganization</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMAIL_TITLE</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户注册组织，发送邮箱验证进行验证</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>IS_ALLOW_CONFIG</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>organization</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>project</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>choerodon验证邮件</t>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>&lt;p&gt;${userName}，您好！&lt;/p&gt;&lt;p&gt;请使用下面的验证码重置您的密码，验证码 10 分钟内有效:&lt;/p&gt;&lt;p&gt; ${verifyCode}&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>停用组织</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>添加新用户</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>修改密码</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>pm</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>addFunction</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>addFunction-preset</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;p&gt;您已经成功添加${addCount}名新用户&lt;/p&gt;</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>${content}</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>系统通知</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>系统通知</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>管理员添加/导入新用户</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>管理员添加或导入新用户时，管理员收到添加用户结果的反馈</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>registerOrganization</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>registerOrganization</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>注册组织</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>forgetPassword-preset</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>registerOrganization-preset</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>enableOrganization</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>验证邮件</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
@@ -2270,35 +2292,7 @@
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
-    <t>registerOrganization</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMAIL_TITLE</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>choerodon</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>choerodon</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户注册组织，发送邮箱验证进行验证</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>IS_ALLOW_CONFIG</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>organization</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>project</t>
+    <t>EMAIL_CONTENT</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
 </sst>
@@ -3265,8 +3259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D7:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3310,7 +3304,7 @@
         <v>63</v>
       </c>
       <c r="M7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="4:13">
@@ -3350,13 +3344,13 @@
         <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I9" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -3443,7 +3437,7 @@
         <v>91</v>
       </c>
       <c r="I12" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -3472,7 +3466,7 @@
         <v>90</v>
       </c>
       <c r="I13" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -3501,7 +3495,7 @@
         <v>92</v>
       </c>
       <c r="I14" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -3530,7 +3524,7 @@
         <v>93</v>
       </c>
       <c r="I15" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -3547,16 +3541,16 @@
     </row>
     <row r="16" spans="4:13">
       <c r="E16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" t="s">
         <v>123</v>
       </c>
-      <c r="G16" t="s">
-        <v>125</v>
-      </c>
       <c r="H16" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I16" t="s">
         <v>47</v>
@@ -3585,8 +3579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D7:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -3600,6 +3594,7 @@
     <col min="11" max="11" width="20.125" customWidth="1"/>
     <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="109.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="134.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="4:18">
@@ -3625,13 +3620,16 @@
         <v>68</v>
       </c>
       <c r="K7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L7" t="s">
         <v>69</v>
       </c>
       <c r="M7" t="s">
         <v>70</v>
+      </c>
+      <c r="N7" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="4:18">
@@ -3696,7 +3694,7 @@
         <v>105</v>
       </c>
       <c r="G10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H10" t="s">
         <v>72</v>
@@ -3731,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L11" t="s">
         <v>74</v>
@@ -3748,7 +3746,7 @@
         <v>103</v>
       </c>
       <c r="G12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H12" t="s">
         <v>72</v>
@@ -3763,7 +3761,7 @@
         <v>102</v>
       </c>
       <c r="M12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="4:18">
@@ -3774,7 +3772,7 @@
         <v>99</v>
       </c>
       <c r="G13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H13" t="s">
         <v>95</v>
@@ -3797,25 +3795,25 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="4:18">
@@ -3823,7 +3821,7 @@
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G15" t="s">
         <v>100</v>
@@ -3840,11 +3838,8 @@
       <c r="K15" t="s">
         <v>133</v>
       </c>
-      <c r="L15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M15" t="s">
-        <v>110</v>
+      <c r="N15" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="4:18">
@@ -3852,10 +3847,10 @@
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H16" t="s">
         <v>108</v>
@@ -3864,16 +3859,13 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K16" t="s">
-        <v>134</v>
-      </c>
-      <c r="L16" t="s">
-        <v>129</v>
-      </c>
-      <c r="M16" t="s">
-        <v>130</v>
+        <v>133</v>
+      </c>
+      <c r="N16" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ADD] init-data.xlsx add sendsetting and station letter template about schedule task status.
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-08-28-init-data.xlsx
+++ b/src/main/resources/script/db/2018-08-28-init-data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DYQ\tranning\choerodon-framework\notify-service\src\main\resources\script\db\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF4294B-6C6A-44B7-8509-B1A57FDD7E5F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19935" windowHeight="7860" tabRatio="452" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19935" windowHeight="7860" tabRatio="452" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -20,14 +26,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="143">
   <si>
     <r>
       <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">注意这个文档不能 </t>
     </r>
@@ -45,7 +51,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>！！
 发现冲突以后，先备份自己的改动，然后更新到最新版，然后再添加新的数据。</t>
@@ -57,7 +63,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">正式的数据从第二个 </t>
     </r>
@@ -75,7 +81,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>页开始</t>
     </r>
@@ -93,7 +99,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">每页 从 </t>
     </r>
@@ -111,7 +117,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">单元格开始有效
 </t>
@@ -121,7 +127,7 @@
         <sz val="12"/>
         <color rgb="FFF4B183"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>同一个表的数据要连续</t>
     </r>
@@ -139,7 +145,7 @@
         <sz val="12"/>
         <color rgb="FFF4B183"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">中间不能有空行
 </t>
@@ -158,7 +164,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>页的名字不要包含空格</t>
     </r>
@@ -176,7 +182,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>中文等</t>
     </r>
@@ -187,7 +193,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>颜色示例</t>
     </r>
@@ -205,7 +211,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>非必须</t>
     </r>
@@ -223,7 +229,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>非强制</t>
     </r>
@@ -244,7 +250,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>请给特殊单元格</t>
     </r>
@@ -264,7 +270,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>列名添加颜色</t>
     </r>
@@ -284,7 +290,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>提高数据可读性</t>
     </r>
@@ -304,7 +310,7 @@
         <sz val="12"/>
         <color rgb="FFC55A11"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>自动生成</t>
     </r>
@@ -324,7 +330,7 @@
         <sz val="12"/>
         <color rgb="FF2E75B6"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>唯一性检查</t>
     </r>
@@ -335,7 +341,7 @@
         <sz val="12"/>
         <color rgb="FF548235"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>公式</t>
     </r>
@@ -353,7 +359,7 @@
         <sz val="12"/>
         <color rgb="FF548235"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>外键引用</t>
     </r>
@@ -364,7 +370,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>理论上</t>
     </r>
@@ -382,7 +388,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>表的前后顺序</t>
     </r>
@@ -400,7 +406,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>页的顺序没有严格要求</t>
     </r>
@@ -418,7 +424,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>但请尽量按照先插 后引用的顺序排列</t>
     </r>
@@ -436,7 +442,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>减少迭代次数</t>
     </r>
@@ -483,7 +489,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>前置</t>
     </r>
@@ -501,7 +507,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>该列的值自动生成</t>
     </r>
@@ -519,7 +525,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>当数据库存在等价记录时</t>
     </r>
@@ -537,7 +543,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>这个值会被替换为数据库中已存在的值</t>
     </r>
@@ -548,7 +554,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>自增长</t>
     </r>
@@ -566,7 +572,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>或序列</t>
     </r>
@@ -584,7 +590,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>主键列</t>
     </r>
@@ -603,7 +609,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>当不作为外键引用时</t>
     </r>
@@ -621,7 +627,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>一般写</t>
     </r>
@@ -640,7 +646,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>作为外键时</t>
     </r>
@@ -658,7 +664,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>写可读的值</t>
     </r>
@@ -669,7 +675,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">目前 </t>
     </r>
@@ -687,7 +693,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>是序列</t>
     </r>
@@ -705,7 +711,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>其他自增涨</t>
     </r>
@@ -728,7 +734,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>前置</t>
     </r>
@@ -746,7 +752,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>表中所有带有</t>
     </r>
@@ -764,7 +770,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>的列组成一个唯一性校验</t>
     </r>
@@ -782,7 +788,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>在执行插入之前</t>
     </r>
@@ -800,7 +806,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>会首先按照唯一键来检查数据库是否存在等价记录</t>
     </r>
@@ -811,7 +817,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>可以有多列</t>
     </r>
@@ -829,7 +835,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>仅支持</t>
     </r>
@@ -839,7 +845,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>数字</t>
     </r>
@@ -859,7 +865,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">字符串
 </t>
@@ -869,7 +875,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>当</t>
     </r>
@@ -887,7 +893,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>列涉及到公式时</t>
     </r>
@@ -905,7 +911,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>会先确定公式的值</t>
     </r>
@@ -928,7 +934,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>指定这一列的类型</t>
     </r>
@@ -946,7 +952,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>默认会自动检测</t>
     </r>
@@ -965,7 +971,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>结尾为数字</t>
     </r>
@@ -984,7 +990,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>结尾为日期</t>
     </r>
@@ -1003,7 +1009,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>其他默认为</t>
     </r>
@@ -1023,7 +1029,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>一般不需要指定</t>
     </r>
@@ -1042,7 +1048,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>日期格式仅支持</t>
     </r>
@@ -1076,7 +1082,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>指定语言环境</t>
     </r>
@@ -1096,7 +1102,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>表数据不需要专门写</t>
     </r>
@@ -1107,7 +1113,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>外键引用</t>
     </r>
@@ -1125,7 +1131,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>公式</t>
     </r>
@@ -1145,6 +1151,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>用于引用外键</t>
@@ -1163,6 +1170,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>也可用于普通值
@@ -1175,6 +1183,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>自动增长列</t>
@@ -1193,6 +1202,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>如果被公式引用</t>
@@ -1211,6 +1221,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>最好写一个人可以读懂的值</t>
@@ -1229,6 +1240,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>增强公式可读性</t>
@@ -1243,7 +1255,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>一般用于引用自动生成的外键</t>
     </r>
@@ -1261,7 +1273,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">所有公式均为 </t>
     </r>
@@ -1279,7 +1291,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>支持的标准公式</t>
     </r>
@@ -1297,7 +1309,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>但不支持特别复杂的计算公式</t>
     </r>
@@ -1315,7 +1327,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>比如范围计算</t>
     </r>
@@ -1330,7 +1342,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>相对</t>
     </r>
@@ -1339,7 +1351,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">引用当前页 </t>
     </r>
@@ -1357,7 +1369,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>单元格</t>
     </r>
@@ -1372,7 +1384,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>绝对</t>
     </r>
@@ -1381,7 +1393,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">引用当前页 </t>
     </r>
@@ -1399,7 +1411,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>单元格</t>
     </r>
@@ -1413,7 +1425,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">引用 </t>
     </r>
@@ -1431,7 +1443,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">页的 </t>
     </r>
@@ -1449,7 +1461,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>单元格</t>
     </r>
@@ -1468,7 +1480,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>相对</t>
     </r>
@@ -1491,7 +1503,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">引用 </t>
     </r>
@@ -1509,7 +1521,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">页的 </t>
     </r>
@@ -1527,7 +1539,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>单元格</t>
     </r>
@@ -1546,7 +1558,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>绝对</t>
     </r>
@@ -1566,7 +1578,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>关于</t>
     </r>
@@ -1576,7 +1588,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>相对</t>
     </r>
@@ -1585,7 +1597,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>引用</t>
     </r>
@@ -1596,7 +1608,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>举例</t>
     </r>
@@ -1614,7 +1626,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">当 </t>
     </r>
@@ -1632,7 +1644,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">单元格引用 </t>
     </r>
@@ -1650,7 +1662,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">时
 将 </t>
@@ -1669,7 +1681,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">的复制到 </t>
     </r>
@@ -1687,7 +1699,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>单元格时</t>
     </r>
@@ -1705,7 +1717,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">引用的是 </t>
     </r>
@@ -1724,7 +1736,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">将 </t>
     </r>
@@ -1742,7 +1754,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">的复制到 </t>
     </r>
@@ -1760,7 +1772,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>时</t>
     </r>
@@ -1778,7 +1790,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">实际引用的是 </t>
     </r>
@@ -1797,7 +1809,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>以上情况适用于拖拽填充</t>
     </r>
@@ -1808,7 +1820,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>关于</t>
     </r>
@@ -1818,7 +1830,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>绝对</t>
     </r>
@@ -1827,7 +1839,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>引用</t>
     </r>
@@ -1838,7 +1850,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>复制公式单元格时</t>
     </r>
@@ -1856,7 +1868,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>保持公式不变</t>
     </r>
@@ -1867,7 +1879,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>相对引用</t>
     </r>
@@ -1885,7 +1897,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>绝对引用各有用途</t>
     </r>
@@ -1904,7 +1916,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK JP Regular"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>直接拖拽填充就可以避免大量重复工作</t>
     </r>
@@ -2157,19 +2169,72 @@
   </si>
   <si>
     <t>organizationNotification-preset</t>
+  </si>
+  <si>
+    <t>平台任务状态通知</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>site</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>组织任务状态通知</t>
+  </si>
+  <si>
+    <t>项目任务状态通知</t>
+  </si>
+  <si>
+    <t>registerOrganization</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>jobStatusSite</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>jobStatusOrganization</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>jobStatusProject</t>
+  </si>
+  <si>
+    <t>jobStatusProject</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>jobStatusSite-preset</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>jobStatusOrganization-preset</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>jobStatusProject-preset</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务状态变更通知</t>
+  </si>
+  <si>
+    <t>${jobName}状态发生变更</t>
+  </si>
+  <si>
+    <t>您好，${userName}。${jobName}任务已${jobStatus}，请注意查看。</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>定时任务状态发生变化，给相关用户发送通知。</t>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="36">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2180,7 +2245,7 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Noto Sans CJK JP Regular"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2199,14 +2264,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK JP Regular"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK JP Regular"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2224,164 +2289,13 @@
       <sz val="12"/>
       <color rgb="FF548235"/>
       <name val="Noto Sans CJK JP Regular"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFF4B183"/>
       <name val="Noto Sans CJK JP Regular"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2399,13 +2313,13 @@
       <sz val="12"/>
       <color rgb="FFC55A11"/>
       <name val="Noto Sans CJK JP Regular"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF2E75B6"/>
       <name val="Noto Sans CJK JP Regular"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2417,10 +2331,22 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="DengXian"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2451,194 +2377,8 @@
         <bgColor rgb="FFE7E6E6"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2739,254 +2479,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="36" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
@@ -2997,155 +2495,108 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="49" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="49" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="49" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="49" applyFont="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="49" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="49" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="49" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="49" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="49" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
-    <cellStyle name="Normal" xfId="49"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
@@ -3218,6 +2669,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3475,267 +2929,266 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="9" style="2"/>
     <col min="3" max="3" width="100.625" customWidth="1"/>
     <col min="4" max="4" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="63.95" customHeight="1" spans="1:8">
+    <row r="1" spans="1:8" ht="63.95" customHeight="1">
       <c r="A1" s="4"/>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2"/>
       <c r="D2"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" ht="48.95" customHeight="1" spans="1:7">
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="48.95" customHeight="1">
       <c r="A3"/>
-      <c r="C3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
+      <c r="C3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" ht="30" spans="1:7">
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" ht="31.5">
       <c r="A4"/>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:8">
       <c r="A5" s="4"/>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="4:4">
+    <row r="6" spans="1:8">
       <c r="D6"/>
     </row>
-    <row r="7" spans="3:5">
-      <c r="C7" s="15" t="s">
+    <row r="7" spans="1:8">
+      <c r="C7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
-      <c r="C8" s="18" t="s">
+    <row r="8" spans="1:8">
+      <c r="C8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="20"/>
-    </row>
-    <row r="9" ht="161.25" spans="3:6">
-      <c r="C9" s="21" t="s">
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" ht="173.25">
+      <c r="C9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="191.25" spans="3:5">
-      <c r="C10" s="24" t="s">
+    <row r="10" spans="1:8" ht="204.75">
+      <c r="C10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" ht="85.5" customHeight="1" spans="3:5">
-      <c r="C11" s="18" t="s">
+    <row r="11" spans="1:8" ht="85.5" customHeight="1">
+      <c r="C11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" ht="44.25" spans="3:5">
-      <c r="C12" s="18" t="s">
+    <row r="12" spans="1:8" ht="47.25">
+      <c r="C12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="3:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="20"/>
-    </row>
-    <row r="14" spans="3:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-    </row>
-    <row r="15" ht="132.75" spans="3:5">
-      <c r="C15" s="26" t="s">
+    <row r="13" spans="1:8">
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:8" ht="132.75">
+      <c r="C15" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="4:4">
+    <row r="16" spans="1:8">
       <c r="D16"/>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="3:5">
       <c r="D17"/>
     </row>
-    <row r="18" spans="3:4">
-      <c r="C18" s="14" t="s">
+    <row r="18" spans="3:5">
+      <c r="C18" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D18"/>
     </row>
     <row r="19" spans="3:5">
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-    </row>
-    <row r="20" spans="3:4">
-      <c r="C20" s="30" t="s">
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+    </row>
+    <row r="20" spans="3:5">
+      <c r="C20" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="3:4">
-      <c r="C21" s="30" t="s">
+    <row r="21" spans="3:5">
+      <c r="C21" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="3:4">
-      <c r="C22" s="30" t="s">
+    <row r="22" spans="3:5">
+      <c r="C22" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="3:4">
-      <c r="C23" s="30" t="s">
+    <row r="23" spans="3:5">
+      <c r="C23" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="3:5">
       <c r="D24"/>
     </row>
-    <row r="25" ht="69" customHeight="1" spans="3:5">
-      <c r="C25" s="32" t="s">
+    <row r="25" spans="3:5" ht="69" customHeight="1">
+      <c r="C25" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" customHeight="1" spans="3:5">
-      <c r="C26" s="19" t="s">
+      <c r="E25" s="30"/>
+    </row>
+    <row r="26" spans="3:5" ht="15.75" customHeight="1">
+      <c r="C26" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" ht="30" spans="3:3">
-      <c r="C27" s="33" t="s">
+      <c r="E26" s="30"/>
+    </row>
+    <row r="27" spans="3:5" ht="31.5">
+      <c r="C27" s="28" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C19:E19"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
   </mergeCells>
-  <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <phoneticPr fontId="17" type="noConversion"/>
+  <pageMargins left="0.69791666666666696" right="0.69791666666666696" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="D7:M18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="D7:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3784,7 +3237,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="5:13">
+    <row r="8" spans="4:13">
       <c r="E8" t="s">
         <v>54</v>
       </c>
@@ -3813,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="5:13">
+    <row r="9" spans="4:13">
       <c r="E9" t="s">
         <v>58</v>
       </c>
@@ -3842,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="5:13">
+    <row r="10" spans="4:13">
       <c r="E10" t="s">
         <v>62</v>
       </c>
@@ -3871,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="5:13">
+    <row r="11" spans="4:13">
       <c r="E11" t="s">
         <v>65</v>
       </c>
@@ -3900,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="5:13">
+    <row r="12" spans="4:13">
       <c r="E12" t="s">
         <v>68</v>
       </c>
@@ -3929,7 +3382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="5:13">
+    <row r="13" spans="4:13">
       <c r="E13" t="s">
         <v>72</v>
       </c>
@@ -3958,7 +3411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="5:13">
+    <row r="14" spans="4:13">
       <c r="E14" t="s">
         <v>75</v>
       </c>
@@ -3987,7 +3440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="5:13">
+    <row r="15" spans="4:13">
       <c r="E15" t="s">
         <v>78</v>
       </c>
@@ -4016,9 +3469,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="5:13">
+    <row r="16" spans="4:13">
       <c r="E16" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="F16" t="s">
         <v>81</v>
@@ -4103,20 +3556,106 @@
         <v>1</v>
       </c>
     </row>
+    <row r="19" spans="5:13">
+      <c r="E19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" t="s">
+        <v>132</v>
+      </c>
+      <c r="G19" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" t="s">
+        <v>142</v>
+      </c>
+      <c r="I19" t="s">
+        <v>128</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13">
+      <c r="E20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I20" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13">
+      <c r="E21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" t="s">
+        <v>142</v>
+      </c>
+      <c r="I21" t="s">
+        <v>71</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="17" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="D7:R18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="D7:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -4125,14 +3664,14 @@
     <col min="6" max="6" width="26.625" customWidth="1"/>
     <col min="7" max="7" width="16.125" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="22.8583333333333" customWidth="1"/>
+    <col min="9" max="9" width="22.875" customWidth="1"/>
     <col min="10" max="11" width="20.125" customWidth="1"/>
     <col min="12" max="12" width="11.625" customWidth="1"/>
     <col min="13" max="13" width="109.375" customWidth="1"/>
     <col min="14" max="14" width="134.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:14">
+    <row r="7" spans="4:18">
       <c r="D7" t="s">
         <v>90</v>
       </c>
@@ -4167,7 +3706,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="5:18">
+    <row r="8" spans="4:18">
       <c r="E8">
         <v>1</v>
       </c>
@@ -4195,7 +3734,7 @@
       <c r="P8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="5:13">
+    <row r="9" spans="4:18">
       <c r="E9">
         <v>2</v>
       </c>
@@ -4221,7 +3760,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="5:13">
+    <row r="10" spans="4:18">
       <c r="E10">
         <v>3</v>
       </c>
@@ -4247,7 +3786,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="5:13">
+    <row r="11" spans="4:18">
       <c r="E11">
         <v>4</v>
       </c>
@@ -4273,7 +3812,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="5:13">
+    <row r="12" spans="4:18">
       <c r="E12">
         <v>5</v>
       </c>
@@ -4299,7 +3838,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="5:13">
+    <row r="13" spans="4:18">
       <c r="E13">
         <v>6</v>
       </c>
@@ -4325,7 +3864,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="5:13">
+    <row r="14" spans="4:18">
       <c r="E14">
         <v>7</v>
       </c>
@@ -4351,7 +3890,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="5:14">
+    <row r="15" spans="4:18">
       <c r="E15">
         <v>8</v>
       </c>
@@ -4377,7 +3916,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="5:14">
+    <row r="16" spans="4:18">
       <c r="E16">
         <v>9</v>
       </c>
@@ -4455,9 +3994,87 @@
         <v>118</v>
       </c>
     </row>
+    <row r="19" spans="5:13">
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" t="s">
+        <v>139</v>
+      </c>
+      <c r="H19" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>132</v>
+      </c>
+      <c r="L19" t="s">
+        <v>140</v>
+      </c>
+      <c r="M19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13">
+      <c r="E20">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>137</v>
+      </c>
+      <c r="G20" t="s">
+        <v>139</v>
+      </c>
+      <c r="H20" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>133</v>
+      </c>
+      <c r="L20" t="s">
+        <v>140</v>
+      </c>
+      <c r="M20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13">
+      <c r="E21">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>135</v>
+      </c>
+      <c r="L21" t="s">
+        <v>140</v>
+      </c>
+      <c r="M21" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <phoneticPr fontId="17" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[ADD] add resource delete template
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-08-28-init-data.xlsx
+++ b/src/main/resources/script/db/2018-08-28-init-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19935" windowHeight="7785" tabRatio="452" activeTab="2"/>
+    <workbookView windowWidth="22391" windowHeight="6912" tabRatio="452" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="149">
   <si>
     <r>
       <rPr>
@@ -2060,6 +2060,15 @@
     <t>当事务实例失败时，向触发者发送消息提醒。</t>
   </si>
   <si>
+    <t>resourceDeleteConfirmation</t>
+  </si>
+  <si>
+    <t>资源删除确认通知</t>
+  </si>
+  <si>
+    <t>删除Devops资源时，给相关用户发送验证码</t>
+  </si>
+  <si>
     <t>NOTIFY_TEMPLATE</t>
   </si>
   <si>
@@ -2193,6 +2202,27 @@
   </si>
   <si>
     <t>&lt;p&gt;您好，${userName}。&lt;/p&gt;&lt;p&gt;您触发事务实例运行失败。&lt;/p&gt;&lt;p&gt;编号:${sagaInstanceId}&lt;/p&gt;&lt;p&gt;所属事务:${sagaCode}&lt;/p&gt;&lt;p&gt;层级:${level}&lt;/p&gt;&lt;p&gt;请自行重试或联系相关管理员&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>resourceDeleteConfirmation-preset</t>
+  </si>
+  <si>
+    <t>resourceDeleteConfirmation-email</t>
+  </si>
+  <si>
+    <t>Choerodon验证邮件</t>
+  </si>
+  <si>
+    <t>您好，${user}正在${env}环境下执行删除${object}"${objectName}"的操作，验证码为：${verificationCode}；确认后，需将此验证码提供给操作者${user}完成删除操作。验证码10分钟内有效。</t>
+  </si>
+  <si>
+    <t>resourceDeleteConfirmation-pm</t>
+  </si>
+  <si>
+    <t>删除操作验证码</t>
+  </si>
+  <si>
+    <t>${user}正在${env}环境下执行删除${object}"${objectName}"的操作，验证码为：${verificationCode}；确认后，需将此验证码提供给操作者${user}完成删除操作。验证码10分钟内有效。</t>
   </si>
 </sst>
 </file>
@@ -2200,10 +2230,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="37">
     <font>
@@ -2270,58 +2300,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2349,9 +2335,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2381,9 +2374,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2405,8 +2405,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2417,6 +2418,35 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2495,7 +2525,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2507,13 +2615,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2525,79 +2681,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2609,73 +2699,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2782,17 +2812,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2816,7 +2840,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2832,11 +2871,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2864,168 +2909,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3531,10 +3561,10 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="2" width="9" style="4"/>
-    <col min="3" max="3" width="100.625" customWidth="1"/>
+    <col min="3" max="3" width="100.628787878788" customWidth="1"/>
     <col min="4" max="4" width="9" style="5"/>
   </cols>
   <sheetData>
@@ -3566,7 +3596,7 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" ht="30" spans="1:7">
+    <row r="4" ht="31.2" spans="1:7">
       <c r="A4"/>
       <c r="C4" s="12" t="s">
         <v>3</v>
@@ -3612,7 +3642,7 @@
       </c>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" ht="161.25" spans="3:6">
+    <row r="9" ht="156" spans="3:6">
       <c r="C9" s="23" t="s">
         <v>13</v>
       </c>
@@ -3626,7 +3656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="191.25" spans="3:5">
+    <row r="10" ht="202.8" spans="3:5">
       <c r="C10" s="26" t="s">
         <v>17</v>
       </c>
@@ -3648,7 +3678,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" ht="44.25" spans="3:5">
+    <row r="12" ht="46.8" spans="3:5">
       <c r="C12" s="20" t="s">
         <v>23</v>
       </c>
@@ -3669,7 +3699,7 @@
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
     </row>
-    <row r="15" ht="132.75" spans="3:5">
+    <row r="15" ht="124.8" spans="3:5">
       <c r="C15" s="28" t="s">
         <v>26</v>
       </c>
@@ -3743,7 +3773,7 @@
       </c>
       <c r="E25" s="10"/>
     </row>
-    <row r="26" customHeight="1" spans="3:5">
+    <row r="26" ht="15.75" customHeight="1" spans="3:5">
       <c r="C26" s="21" t="s">
         <v>41</v>
       </c>
@@ -3752,7 +3782,7 @@
       </c>
       <c r="E26" s="10"/>
     </row>
-    <row r="27" ht="30" spans="3:3">
+    <row r="27" ht="31.2" spans="3:3">
       <c r="C27" s="35" t="s">
         <v>43</v>
       </c>
@@ -3776,23 +3806,23 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D7:M20"/>
+  <dimension ref="D7:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="$A10:$XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="D7:M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="3" max="3" width="5.75" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="4" max="4" width="16.1287878787879" customWidth="1"/>
     <col min="5" max="5" width="22.5" customWidth="1"/>
-    <col min="6" max="6" width="20.125" customWidth="1"/>
-    <col min="7" max="7" width="17.625" customWidth="1"/>
+    <col min="6" max="6" width="20.1287878787879" customWidth="1"/>
+    <col min="7" max="7" width="17.6287878787879" customWidth="1"/>
     <col min="8" max="8" width="32.75" customWidth="1"/>
-    <col min="10" max="10" width="14.875" customWidth="1"/>
-    <col min="11" max="11" width="20.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="10" max="10" width="14.8787878787879" customWidth="1"/>
+    <col min="11" max="11" width="20.3787878787879" customWidth="1"/>
+    <col min="12" max="12" width="14.6287878787879" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4202,6 +4232,35 @@
         <v>1</v>
       </c>
       <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13">
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
         <v>1</v>
       </c>
     </row>
@@ -4215,29 +4274,29 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D7:R20"/>
+  <dimension ref="D7:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F24" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.87878787878788" defaultRowHeight="15.6"/>
   <cols>
-    <col min="4" max="4" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="18.8787878787879" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="26.625" customWidth="1"/>
-    <col min="7" max="7" width="16.125" customWidth="1"/>
+    <col min="6" max="6" width="26.6287878787879" customWidth="1"/>
+    <col min="7" max="7" width="16.1287878787879" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="22.875" customWidth="1"/>
-    <col min="10" max="11" width="20.125" customWidth="1"/>
-    <col min="12" max="12" width="28.625" customWidth="1"/>
-    <col min="13" max="13" width="109.375" customWidth="1"/>
-    <col min="14" max="14" width="134.625" customWidth="1"/>
+    <col min="9" max="9" width="22.8787878787879" customWidth="1"/>
+    <col min="10" max="11" width="20.1287878787879" customWidth="1"/>
+    <col min="12" max="12" width="28.6287878787879" customWidth="1"/>
+    <col min="13" max="13" width="109.378787878788" customWidth="1"/>
+    <col min="14" max="14" width="134.628787878788" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="4:14">
       <c r="D7" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
@@ -4249,39 +4308,39 @@
         <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="K7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="L7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="M7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="5:18">
       <c r="E8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G8" t="s">
         <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -4290,26 +4349,26 @@
         <v>65</v>
       </c>
       <c r="L8" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="M8" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="P8" s="2"/>
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="5:13">
       <c r="E9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G9" t="s">
         <v>70</v>
       </c>
       <c r="H9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -4318,24 +4377,24 @@
         <v>69</v>
       </c>
       <c r="L9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="M9" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="5:13">
       <c r="E10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G10" t="s">
         <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -4344,24 +4403,24 @@
         <v>75</v>
       </c>
       <c r="L10" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="M10" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="5:13">
       <c r="E11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G11" t="s">
         <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -4370,24 +4429,24 @@
         <v>72</v>
       </c>
       <c r="L11" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="M11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="5:13">
       <c r="E12" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F12" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H12" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -4396,24 +4455,24 @@
         <v>58</v>
       </c>
       <c r="L12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="M12" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="5:13">
       <c r="E13" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F13" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G13" t="s">
         <v>63</v>
       </c>
       <c r="H13" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -4425,47 +4484,47 @@
         <v>63</v>
       </c>
       <c r="M13" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="5:13">
       <c r="E14" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F14" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G14" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H14" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L14" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="M14" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="5:14">
       <c r="E15" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F15" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G15" t="s">
         <v>55</v>
       </c>
       <c r="H15" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -4474,24 +4533,24 @@
         <v>54</v>
       </c>
       <c r="K15" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="N15" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="5:14">
       <c r="E16" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F16" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G16" t="s">
         <v>79</v>
       </c>
       <c r="H16" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -4500,24 +4559,24 @@
         <v>78</v>
       </c>
       <c r="K16" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="N16" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="5:13">
       <c r="E17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H17" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -4526,24 +4585,24 @@
         <v>81</v>
       </c>
       <c r="L17" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="M17" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="5:13">
       <c r="E18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" t="s">
+        <v>137</v>
+      </c>
+      <c r="G18" t="s">
         <v>134</v>
       </c>
-      <c r="F18" t="s">
-        <v>134</v>
-      </c>
-      <c r="G18" t="s">
-        <v>131</v>
-      </c>
       <c r="H18" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -4552,24 +4611,24 @@
         <v>84</v>
       </c>
       <c r="L18" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="M18" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="5:13">
       <c r="E19" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F19" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G19" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H19" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -4578,24 +4637,24 @@
         <v>86</v>
       </c>
       <c r="L19" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="M19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" ht="31.5" spans="5:13">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" ht="31.2" spans="5:13">
       <c r="E20" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F20" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H20" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -4604,10 +4663,63 @@
         <v>91</v>
       </c>
       <c r="L20" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="5:14">
+      <c r="E21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>94</v>
+      </c>
+      <c r="K21" t="s">
+        <v>144</v>
+      </c>
+      <c r="N21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="5:13">
+      <c r="E22" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>94</v>
+      </c>
+      <c r="K22"/>
+      <c r="L22" t="s">
+        <v>147</v>
+      </c>
+      <c r="M22" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>